<commit_message>
added bindings + sample chai (problem with scaling) + updated explanations
</commit_message>
<xml_diff>
--- a/Chaiscripts/Explanation_checkered.xlsx
+++ b/Chaiscripts/Explanation_checkered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wannes\Documents\3dcg1819-team\Chaiscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E4E1E1-1919-4265-98A9-16C6ACEA69BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415EBC81-2862-42B5-9F6E-D7E803CCB681}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8790" xr2:uid="{AA2B0F1E-7ADF-44B2-9E94-620D8E4BF785}"/>
   </bookViews>
@@ -131,17 +131,17 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53B9D74-D024-479E-B8D2-B14EEE35542F}">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -472,50 +472,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
         <f>B1+1</f>
         <v>2</v>
       </c>
-      <c r="D1" s="3">
-        <f t="shared" ref="D1:P1" si="0">C1+1</f>
+      <c r="D1" s="1">
+        <f t="shared" ref="D1:J1" si="0">C1+1</f>
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
@@ -528,15 +528,15 @@
       </c>
       <c r="D2">
         <f>U33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>U43</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>U53</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f>U63</f>
@@ -544,35 +544,35 @@
       </c>
       <c r="H2">
         <f>U73</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>U83</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <f>U93</f>
         <v>1</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="S2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="S2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" si="1">U14</f>
+        <f t="shared" ref="B3:B10" si="1">U14</f>
         <v>0</v>
       </c>
       <c r="C3">
@@ -581,58 +581,58 @@
       </c>
       <c r="D3">
         <f>U34</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f>U44</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>U54</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="2">U64</f>
+        <f t="shared" ref="G3:G10" si="2">U64</f>
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H11" si="3">U74</f>
-        <v>0</v>
+        <f t="shared" ref="H3:H10" si="3">U74</f>
+        <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="4">U84</f>
-        <v>1</v>
+        <f t="shared" ref="I3:I10" si="4">U84</f>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J11" si="5">U94</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
+        <f t="shared" ref="J3:J10" si="5">U94</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
       <c r="S3" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="1"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <f t="shared" ref="A4:A16" si="6">A3+1</f>
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A10" si="6">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>U25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f>U35</f>
@@ -644,11 +644,11 @@
       </c>
       <c r="F4">
         <f>U55</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
@@ -660,34 +660,34 @@
       </c>
       <c r="J4">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
       <c r="S4" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="2"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>U26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>U36</f>
@@ -699,11 +699,11 @@
       </c>
       <c r="F5">
         <f>U56</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
@@ -715,19 +715,19 @@
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -741,11 +741,11 @@
       </c>
       <c r="D6">
         <f>U37</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>U47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f>U57</f>
@@ -757,28 +757,28 @@
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
       <c r="S6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -787,19 +787,19 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C11" si="7">U28</f>
+        <f t="shared" ref="C7:C10" si="7">U28</f>
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D11" si="8">U38</f>
-        <v>0</v>
+        <f t="shared" ref="D7:D10" si="8">U38</f>
+        <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E11" si="9">U48</f>
-        <v>1</v>
+        <f t="shared" ref="E7:E10" si="9">U48</f>
+        <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F11" si="10">U58</f>
+        <f t="shared" ref="F7:F10" si="10">U58</f>
         <v>0</v>
       </c>
       <c r="G7">
@@ -808,38 +808,38 @@
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
       <c r="S7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="8"/>
@@ -851,11 +851,11 @@
       </c>
       <c r="F8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
@@ -867,30 +867,30 @@
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
       <c r="S8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="8"/>
@@ -902,11 +902,11 @@
       </c>
       <c r="F9">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
@@ -918,23 +918,23 @@
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
       <c r="S9" t="s">
         <v>4</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
@@ -948,11 +948,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="10"/>
@@ -964,124 +964,124 @@
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
       <c r="R11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
       <c r="Q12" t="s">
         <v>10</v>
       </c>
       <c r="R12" t="s">
         <v>11</v>
       </c>
-      <c r="W12" s="4"/>
+      <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="6">
-        <v>1</v>
-      </c>
-      <c r="R13" s="4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="4">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
         <v>1</v>
       </c>
       <c r="S13">
         <f>MOD(ROUNDDOWN((Q13/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <f>MOD(ROUNDDOWN((R13/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13">
         <f>IF(S13=T13,1,0)</f>
         <v>1</v>
       </c>
-      <c r="W13" s="4"/>
+      <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="6">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="4">
         <f>$Q$13</f>
         <v>1</v>
       </c>
@@ -1091,36 +1091,36 @@
       </c>
       <c r="S14">
         <f t="shared" ref="S14:S17" si="11">MOD(ROUNDDOWN((Q14/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <f t="shared" ref="T14:T17" si="12">MOD(ROUNDDOWN((R14/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <f t="shared" ref="U14:U32" si="13">IF(S14=T14,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W14" s="4"/>
+        <f t="shared" ref="U14:U17" si="13">IF(S14=T14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="6">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="4">
         <f t="shared" ref="Q15:Q22" si="14">$Q$13</f>
         <v>1</v>
       </c>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <f t="shared" si="12"/>
@@ -1138,28 +1138,28 @@
       </c>
       <c r="U15">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="W15" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="6">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <f t="shared" si="12"/>
@@ -1177,28 +1177,28 @@
       </c>
       <c r="U16">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="W16" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="6">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1208,36 +1208,36 @@
       </c>
       <c r="S17">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="W17" s="4"/>
+      <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="6">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1247,36 +1247,36 @@
       </c>
       <c r="S18">
         <f>MOD(ROUNDDOWN((Q18/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <f>MOD(ROUNDDOWN((R18/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18">
         <f>IF(S18=T18,1,0)</f>
         <v>0</v>
       </c>
-      <c r="W18" s="4"/>
+      <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="6">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="S19">
         <f t="shared" ref="S19:S22" si="16">MOD(ROUNDDOWN((Q19/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <f t="shared" ref="T19:T22" si="17">MOD(ROUNDDOWN((R19/$T$9),0),2)</f>
@@ -1294,27 +1294,27 @@
       </c>
       <c r="U19">
         <f t="shared" ref="U19:U22" si="18">IF(S19=T19,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <f t="shared" si="17"/>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="U20">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="6">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1362,11 +1362,11 @@
       </c>
       <c r="S21">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21">
         <f t="shared" si="18"/>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q22" s="6">
+      <c r="Q22" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
@@ -1384,11 +1384,11 @@
       </c>
       <c r="S22">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
         <f t="shared" si="18"/>
@@ -1400,24 +1400,24 @@
         <f>$Q$13+1</f>
         <v>2</v>
       </c>
-      <c r="R23" s="4">
+      <c r="R23" s="2">
         <v>1</v>
       </c>
       <c r="S23">
         <f>MOD(ROUNDDOWN((Q23/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23">
         <f>MOD(ROUNDDOWN((R23/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23">
-        <f>IF(S23=T23,1,0)</f>
+        <f t="shared" ref="U23:U52" si="19">IF(S23=T23,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q24" s="6">
+      <c r="Q24" s="4">
         <f>$Q$23</f>
         <v>2</v>
       </c>
@@ -1426,191 +1426,191 @@
         <v>2</v>
       </c>
       <c r="S24">
-        <f t="shared" ref="S24:S27" si="19">MOD(ROUNDDOWN((Q24/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="S24:S27" si="20">MOD(ROUNDDOWN((Q24/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="T24">
-        <f t="shared" ref="T24:T27" si="20">MOD(ROUNDDOWN((R24/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T24:T27" si="21">MOD(ROUNDDOWN((R24/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U24">
-        <f>IF(S24=T24,1,0)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q25" s="6">
-        <f t="shared" ref="Q25:Q32" si="21">$Q$23</f>
+      <c r="Q25" s="4">
+        <f t="shared" ref="Q25:Q32" si="22">$Q$23</f>
         <v>2</v>
       </c>
       <c r="R25">
-        <f t="shared" ref="R25:R32" si="22">R24+1</f>
+        <f t="shared" ref="R25:R32" si="23">R24+1</f>
         <v>3</v>
       </c>
       <c r="S25">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q26" s="4">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="S26">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="U25">
-        <f>IF(S25=T25,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q26" s="6">
+      <c r="T26">
         <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q27" s="4">
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="R26">
+      <c r="R27">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q28" s="4">
         <f t="shared" si="22"/>
-        <v>4</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <f>IF(S26=T26,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q27" s="6">
-        <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="R27">
-        <f t="shared" si="22"/>
-        <v>5</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="U27">
-        <f>IF(S27=T27,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q28" s="6">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
       <c r="R28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="S28">
         <f>MOD(ROUNDDOWN((Q28/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28">
         <f>MOD(ROUNDDOWN((R28/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28">
-        <f>IF(S28=T28,1,0)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q29" s="6">
-        <f t="shared" si="21"/>
+      <c r="Q29" s="4">
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="R29">
+        <f t="shared" si="23"/>
+        <v>7</v>
+      </c>
+      <c r="S29">
+        <f t="shared" ref="S29:S32" si="24">MOD(ROUNDDOWN((Q29/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f t="shared" ref="T29:T32" si="25">MOD(ROUNDDOWN((R29/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q30" s="4">
         <f t="shared" si="22"/>
-        <v>7</v>
-      </c>
-      <c r="S29">
-        <f t="shared" ref="S29:S32" si="23">MOD(ROUNDDOWN((Q29/$T$9),0),2)</f>
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <f t="shared" ref="T29:T32" si="24">MOD(ROUNDDOWN((R29/$T$9),0),2)</f>
-        <v>1</v>
-      </c>
-      <c r="U29">
-        <f>IF(S29=T29,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q30" s="6">
-        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="R30">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q31" s="4">
         <f t="shared" si="22"/>
-        <v>8</v>
-      </c>
-      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="R31">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T30">
+        <v>9</v>
+      </c>
+      <c r="S31">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <f>IF(S30=T30,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q31" s="6">
-        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q32" s="4">
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="R31">
-        <f t="shared" si="22"/>
-        <v>9</v>
-      </c>
-      <c r="S31">
+      <c r="R32">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T31">
+        <v>10</v>
+      </c>
+      <c r="S32">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="U31">
-        <f>IF(S31=T31,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q32" s="6">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="22"/>
-        <v>10</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
       <c r="T32">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>1</v>
       </c>
       <c r="U32">
-        <f>IF(S32=T32,1,0)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
         <f>$Q$23+1</f>
         <v>3</v>
       </c>
-      <c r="R33" s="4">
+      <c r="R33" s="2">
         <v>1</v>
       </c>
       <c r="S33">
@@ -1628,15 +1628,15 @@
       </c>
       <c r="T33">
         <f>MOD(ROUNDDOWN((R33/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U33">
-        <f>IF(S33=T33,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="7">
+      <c r="Q34" s="5">
         <f>$Q$33</f>
         <v>3</v>
       </c>
@@ -1645,91 +1645,91 @@
         <v>2</v>
       </c>
       <c r="S34">
-        <f t="shared" ref="S34:S37" si="25">MOD(ROUNDDOWN((Q34/$T$9),0),2)</f>
+        <f t="shared" ref="S34:S37" si="26">MOD(ROUNDDOWN((Q34/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="T34">
-        <f t="shared" ref="T34:T37" si="26">MOD(ROUNDDOWN((R34/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T34:T37" si="27">MOD(ROUNDDOWN((R34/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U34">
-        <f>IF(S34=T34,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="7">
-        <f t="shared" ref="Q35:Q42" si="27">$Q$33</f>
+      <c r="Q35" s="5">
+        <f t="shared" ref="Q35:Q42" si="28">$Q$33</f>
         <v>3</v>
       </c>
       <c r="R35">
-        <f t="shared" ref="R35:R42" si="28">R34+1</f>
+        <f t="shared" ref="R35:R42" si="29">R34+1</f>
         <v>3</v>
       </c>
       <c r="S35">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="T35">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q36" s="5">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="S36">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="U35">
-        <f>IF(S35=T35,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="7">
+      <c r="T36">
         <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q37" s="5">
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
-      <c r="R36">
+      <c r="R37">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q38" s="5">
         <f t="shared" si="28"/>
-        <v>4</v>
-      </c>
-      <c r="S36">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <f>IF(S36=T36,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="7">
-        <f t="shared" si="27"/>
         <v>3</v>
       </c>
-      <c r="R37">
-        <f t="shared" si="28"/>
-        <v>5</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="T37">
-        <f t="shared" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="U37">
-        <f>IF(S37=T37,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="7">
-        <f t="shared" si="27"/>
-        <v>3</v>
-      </c>
       <c r="R38">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="S38">
@@ -1738,99 +1738,99 @@
       </c>
       <c r="T38">
         <f>MOD(ROUNDDOWN((R38/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38">
-        <f>IF(S38=T38,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="7">
-        <f t="shared" si="27"/>
+      <c r="Q39" s="5">
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="R39">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="S39">
+        <f t="shared" ref="S39:S42" si="30">MOD(ROUNDDOWN((Q39/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <f t="shared" ref="T39:T42" si="31">MOD(ROUNDDOWN((R39/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q40" s="5">
         <f t="shared" si="28"/>
-        <v>7</v>
-      </c>
-      <c r="S39">
-        <f t="shared" ref="S39:S42" si="29">MOD(ROUNDDOWN((Q39/$T$9),0),2)</f>
-        <v>1</v>
-      </c>
-      <c r="T39">
-        <f t="shared" ref="T39:T42" si="30">MOD(ROUNDDOWN((R39/$T$9),0),2)</f>
-        <v>1</v>
-      </c>
-      <c r="U39">
-        <f>IF(S39=T39,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="7">
-        <f t="shared" si="27"/>
         <v>3</v>
       </c>
       <c r="R40">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q41" s="5">
         <f t="shared" si="28"/>
-        <v>8</v>
-      </c>
-      <c r="S40">
+        <v>3</v>
+      </c>
+      <c r="R41">
         <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="T40">
+        <v>9</v>
+      </c>
+      <c r="S41">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="U40">
-        <f>IF(S40=T40,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="7">
-        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q42" s="5">
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
-      <c r="R41">
-        <f t="shared" si="28"/>
-        <v>9</v>
-      </c>
-      <c r="S41">
+      <c r="R42">
         <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="T41">
+        <v>10</v>
+      </c>
+      <c r="S42">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="U41">
-        <f>IF(S41=T41,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="7">
-        <f t="shared" si="27"/>
-        <v>3</v>
-      </c>
-      <c r="R42">
-        <f t="shared" si="28"/>
-        <v>10</v>
-      </c>
-      <c r="S42">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
       <c r="T42">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>1</v>
       </c>
       <c r="U42">
-        <f>IF(S42=T42,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
         <f>$Q$33+1</f>
         <v>4</v>
       </c>
-      <c r="R43" s="4">
+      <c r="R43" s="2">
         <v>1</v>
       </c>
       <c r="S43">
@@ -1847,11 +1847,11 @@
       </c>
       <c r="T43">
         <f>MOD(ROUNDDOWN((R43/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U43">
-        <f>IF(S43=T43,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
@@ -1864,91 +1864,91 @@
         <v>2</v>
       </c>
       <c r="S44">
-        <f t="shared" ref="S44:S47" si="31">MOD(ROUNDDOWN((Q44/$T$9),0),2)</f>
+        <f t="shared" ref="S44:S47" si="32">MOD(ROUNDDOWN((Q44/$T$9),0),2)</f>
         <v>0</v>
       </c>
       <c r="T44">
-        <f t="shared" ref="T44:T47" si="32">MOD(ROUNDDOWN((R44/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T44:T47" si="33">MOD(ROUNDDOWN((R44/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U44">
-        <f>IF(S44=T44,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q45">
-        <f t="shared" ref="Q45:Q53" si="33">$Q$43</f>
+        <f t="shared" ref="Q45:Q53" si="34">$Q$43</f>
         <v>4</v>
       </c>
       <c r="R45">
-        <f t="shared" ref="R45:R52" si="34">R44+1</f>
+        <f t="shared" ref="R45:R52" si="35">R44+1</f>
         <v>3</v>
       </c>
       <c r="S45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T45">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="U45">
-        <f>IF(S45=T45,1,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q46">
-        <f t="shared" si="33"/>
-        <v>4</v>
-      </c>
-      <c r="R46">
         <f t="shared" si="34"/>
         <v>4</v>
       </c>
+      <c r="R46">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
       <c r="S46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T46">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="U46">
-        <f>IF(S46=T46,1,0)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q47">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="T47">
         <f t="shared" si="33"/>
-        <v>4</v>
-      </c>
-      <c r="R47">
-        <f t="shared" si="34"/>
-        <v>5</v>
-      </c>
-      <c r="S47">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47">
-        <f>IF(S47=T47,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q48">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="S48">
@@ -1957,107 +1957,107 @@
       </c>
       <c r="T48">
         <f>MOD(ROUNDDOWN((R48/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48">
-        <f>IF(S48=T48,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q49">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R49">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="S49">
-        <f t="shared" ref="S49:S52" si="35">MOD(ROUNDDOWN((Q49/$T$9),0),2)</f>
+        <f t="shared" ref="S49:S52" si="36">MOD(ROUNDDOWN((Q49/$T$9),0),2)</f>
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T49:T52" si="36">MOD(ROUNDDOWN((R49/$T$9),0),2)</f>
+        <f t="shared" ref="T49:T52" si="37">MOD(ROUNDDOWN((R49/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="U49">
-        <f>IF(S49=T49,1,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q50">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R50">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8</v>
       </c>
       <c r="S50">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T50">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="U50">
-        <f>IF(S50=T50,1,0)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q51">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R51">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9</v>
       </c>
       <c r="S51">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T51">
-        <f t="shared" si="36"/>
-        <v>1</v>
+        <f t="shared" si="37"/>
+        <v>0</v>
       </c>
       <c r="U51">
-        <f>IF(S51=T51,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q52">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R52">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="S52">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T52">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <f t="shared" si="37"/>
+        <v>1</v>
       </c>
       <c r="U52">
-        <f>IF(S52=T52,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q53">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
-      <c r="R53" s="4">
+      <c r="R53" s="2">
         <v>1</v>
       </c>
       <c r="S53">
@@ -2066,11 +2066,11 @@
       </c>
       <c r="T53">
         <f>MOD(ROUNDDOWN((R53/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U53">
-        <f t="shared" ref="U53:U57" si="37">IF(S53=T53,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="U53:U57" si="38">IF(S53=T53,1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="17:21" x14ac:dyDescent="0.25">
@@ -2083,15 +2083,15 @@
         <v>2</v>
       </c>
       <c r="S54">
-        <f t="shared" ref="S54:S57" si="38">MOD(ROUNDDOWN((Q54/$T$9),0),2)</f>
-        <v>1</v>
+        <f t="shared" ref="S54:S57" si="39">MOD(ROUNDDOWN((Q54/$T$9),0),2)</f>
+        <v>0</v>
       </c>
       <c r="T54">
-        <f t="shared" ref="T54:T57" si="39">MOD(ROUNDDOWN((R54/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T54:T57" si="40">MOD(ROUNDDOWN((R54/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U54">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -2101,191 +2101,191 @@
         <v>5</v>
       </c>
       <c r="R55">
-        <f t="shared" ref="R55:R62" si="40">R54+1</f>
+        <f t="shared" ref="R55:R62" si="41">R54+1</f>
         <v>3</v>
       </c>
       <c r="S55">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="U55">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="T55">
-        <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="U55">
-        <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q56">
-        <f t="shared" ref="Q56:Q62" si="41">$Q$54</f>
+        <f t="shared" ref="Q56:Q62" si="42">$Q$54</f>
         <v>5</v>
       </c>
       <c r="R56">
+        <f t="shared" si="41"/>
+        <v>4</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="T56">
         <f t="shared" si="40"/>
-        <v>4</v>
-      </c>
-      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="U56">
         <f t="shared" si="38"/>
         <v>1</v>
-      </c>
-      <c r="T56">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="U56">
-        <f t="shared" si="37"/>
-        <v>0</v>
       </c>
     </row>
     <row r="57" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q57">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R57">
         <f t="shared" si="41"/>
         <v>5</v>
       </c>
-      <c r="R57">
+      <c r="S57">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="40"/>
-        <v>5</v>
-      </c>
-      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="U57">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="T57">
-        <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="U57">
-        <f t="shared" si="37"/>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q58">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R58">
         <f t="shared" si="41"/>
-        <v>5</v>
-      </c>
-      <c r="R58">
-        <f t="shared" si="40"/>
         <v>6</v>
       </c>
       <c r="S58">
         <f>MOD(ROUNDDOWN((Q58/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T58">
         <f>MOD(ROUNDDOWN((R58/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U58">
-        <f t="shared" ref="U58:U62" si="42">IF(S58=T58,1,0)</f>
+        <f t="shared" ref="U58:U62" si="43">IF(S58=T58,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q59">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R59">
         <f t="shared" si="41"/>
-        <v>5</v>
-      </c>
-      <c r="R59">
-        <f t="shared" si="40"/>
         <v>7</v>
       </c>
       <c r="S59">
-        <f t="shared" ref="S59:S62" si="43">MOD(ROUNDDOWN((Q59/$T$9),0),2)</f>
-        <v>1</v>
+        <f t="shared" ref="S59:S62" si="44">MOD(ROUNDDOWN((Q59/$T$9),0),2)</f>
+        <v>0</v>
       </c>
       <c r="T59">
-        <f t="shared" ref="T59:T62" si="44">MOD(ROUNDDOWN((R59/$T$9),0),2)</f>
+        <f t="shared" ref="T59:T62" si="45">MOD(ROUNDDOWN((R59/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="U59">
-        <f t="shared" si="42"/>
-        <v>1</v>
+        <f t="shared" si="43"/>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q60">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R60">
         <f t="shared" si="41"/>
-        <v>5</v>
-      </c>
-      <c r="R60">
-        <f t="shared" si="40"/>
         <v>8</v>
       </c>
       <c r="S60">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U60">
         <f t="shared" si="43"/>
         <v>1</v>
-      </c>
-      <c r="T60">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="U60">
-        <f t="shared" si="42"/>
-        <v>0</v>
       </c>
     </row>
     <row r="61" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q61">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R61">
         <f t="shared" si="41"/>
-        <v>5</v>
-      </c>
-      <c r="R61">
-        <f t="shared" si="40"/>
         <v>9</v>
       </c>
       <c r="S61">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U61">
         <f t="shared" si="43"/>
-        <v>1</v>
-      </c>
-      <c r="T61">
-        <f t="shared" si="44"/>
-        <v>1</v>
-      </c>
-      <c r="U61">
-        <f t="shared" si="42"/>
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q62">
+        <f t="shared" si="42"/>
+        <v>5</v>
+      </c>
+      <c r="R62">
         <f t="shared" si="41"/>
-        <v>5</v>
-      </c>
-      <c r="R62">
-        <f t="shared" si="40"/>
         <v>10</v>
       </c>
       <c r="S62">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="45"/>
+        <v>1</v>
+      </c>
+      <c r="U62">
         <f t="shared" si="43"/>
-        <v>1</v>
-      </c>
-      <c r="T62">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="U62">
-        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q63" s="6">
+      <c r="Q63" s="4">
         <f>$Q$54+1</f>
         <v>6</v>
       </c>
-      <c r="R63" s="4">
+      <c r="R63" s="2">
         <v>1</v>
       </c>
       <c r="S63">
         <f>MOD(ROUNDDOWN((Q63/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63">
         <f>MOD(ROUNDDOWN((R63/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63">
         <f>IF(S63=T63,1,0)</f>
@@ -2293,7 +2293,7 @@
       </c>
     </row>
     <row r="64" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q64" s="6">
+      <c r="Q64" s="4">
         <f>$Q$63</f>
         <v>6</v>
       </c>
@@ -2302,100 +2302,100 @@
         <v>2</v>
       </c>
       <c r="S64">
-        <f t="shared" ref="S64:S67" si="45">MOD(ROUNDDOWN((Q64/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="S64:S67" si="46">MOD(ROUNDDOWN((Q64/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="T64">
-        <f t="shared" ref="T64:T67" si="46">MOD(ROUNDDOWN((R64/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T64:T67" si="47">MOD(ROUNDDOWN((R64/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U64">
-        <f t="shared" ref="U64:U67" si="47">IF(S64=T64,1,0)</f>
+        <f t="shared" ref="U64:U67" si="48">IF(S64=T64,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q65" s="6">
-        <f t="shared" ref="Q65:Q72" si="48">$Q$63</f>
+      <c r="Q65" s="4">
+        <f t="shared" ref="Q65:Q72" si="49">$Q$63</f>
         <v>6</v>
       </c>
       <c r="R65">
-        <f t="shared" ref="R65:R72" si="49">R64+1</f>
+        <f t="shared" ref="R65:R72" si="50">R64+1</f>
         <v>3</v>
       </c>
       <c r="S65">
-        <f t="shared" si="45"/>
-        <v>0</v>
+        <f t="shared" si="46"/>
+        <v>1</v>
       </c>
       <c r="T65">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="U65">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="48"/>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="6">
-        <f t="shared" si="48"/>
-        <v>6</v>
-      </c>
-      <c r="R66">
-        <f t="shared" si="49"/>
-        <v>4</v>
-      </c>
-      <c r="S66">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="T66">
-        <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U66">
-        <f t="shared" si="47"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="6">
-        <f t="shared" si="48"/>
-        <v>6</v>
-      </c>
-      <c r="R67">
-        <f t="shared" si="49"/>
-        <v>5</v>
-      </c>
-      <c r="S67">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="T67">
-        <f t="shared" si="46"/>
-        <v>1</v>
-      </c>
-      <c r="U67">
-        <f t="shared" si="47"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="6">
-        <f t="shared" si="48"/>
-        <v>6</v>
-      </c>
-      <c r="R68">
+      <c r="Q66" s="4">
         <f t="shared" si="49"/>
         <v>6</v>
       </c>
+      <c r="R66">
+        <f t="shared" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q67" s="4">
+        <f t="shared" si="49"/>
+        <v>6</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="50"/>
+        <v>5</v>
+      </c>
+      <c r="S67">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="U67">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q68" s="4">
+        <f t="shared" si="49"/>
+        <v>6</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
       <c r="S68">
         <f>MOD(ROUNDDOWN((Q68/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T68">
         <f>MOD(ROUNDDOWN((R68/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U68">
         <f>IF(S68=T68,1,0)</f>
@@ -2403,90 +2403,90 @@
       </c>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="6">
-        <f t="shared" si="48"/>
+      <c r="Q69" s="4">
+        <f t="shared" si="49"/>
         <v>6</v>
       </c>
       <c r="R69">
+        <f t="shared" si="50"/>
+        <v>7</v>
+      </c>
+      <c r="S69">
+        <f t="shared" ref="S69:S72" si="51">MOD(ROUNDDOWN((Q69/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="T69">
+        <f t="shared" ref="T69:T72" si="52">MOD(ROUNDDOWN((R69/$T$9),0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="U69">
+        <f t="shared" ref="U69:U72" si="53">IF(S69=T69,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q70" s="4">
         <f t="shared" si="49"/>
-        <v>7</v>
-      </c>
-      <c r="S69">
-        <f t="shared" ref="S69:S72" si="50">MOD(ROUNDDOWN((Q69/$T$9),0),2)</f>
-        <v>0</v>
-      </c>
-      <c r="T69">
-        <f t="shared" ref="T69:T72" si="51">MOD(ROUNDDOWN((R69/$T$9),0),2)</f>
-        <v>1</v>
-      </c>
-      <c r="U69">
-        <f t="shared" ref="U69:U72" si="52">IF(S69=T69,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="6">
-        <f t="shared" si="48"/>
         <v>6</v>
       </c>
       <c r="R70">
+        <f t="shared" si="50"/>
+        <v>8</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q71" s="4">
         <f t="shared" si="49"/>
-        <v>8</v>
-      </c>
-      <c r="S70">
+        <v>6</v>
+      </c>
+      <c r="R71">
         <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="T70">
+        <v>9</v>
+      </c>
+      <c r="S71">
         <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="U70">
+        <v>1</v>
+      </c>
+      <c r="T71">
         <f t="shared" si="52"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="6">
-        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q72" s="4">
+        <f t="shared" si="49"/>
         <v>6</v>
       </c>
-      <c r="R71">
-        <f t="shared" si="49"/>
-        <v>9</v>
-      </c>
-      <c r="S71">
+      <c r="R72">
         <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="T71">
+        <v>10</v>
+      </c>
+      <c r="S72">
         <f t="shared" si="51"/>
         <v>1</v>
       </c>
-      <c r="U71">
+      <c r="T72">
         <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="6">
-        <f t="shared" si="48"/>
-        <v>6</v>
-      </c>
-      <c r="R72">
-        <f t="shared" si="49"/>
-        <v>10</v>
-      </c>
-      <c r="S72">
-        <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="T72">
-        <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U72">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
         <f>$Q$63+1</f>
         <v>7</v>
       </c>
-      <c r="R73" s="4">
+      <c r="R73" s="2">
         <v>1</v>
       </c>
       <c r="S73">
@@ -2504,11 +2504,11 @@
       </c>
       <c r="T73">
         <f>MOD(ROUNDDOWN((R73/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U73">
-        <f>IF(S73=T73,1,0)</f>
-        <v>1</v>
+        <f t="shared" ref="U73:U102" si="54">IF(S73=T73,1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="17:21" x14ac:dyDescent="0.25">
@@ -2521,91 +2521,91 @@
         <v>2</v>
       </c>
       <c r="S74">
-        <f t="shared" ref="S74:S77" si="53">MOD(ROUNDDOWN((Q74/$T$9),0),2)</f>
+        <f t="shared" ref="S74:S77" si="55">MOD(ROUNDDOWN((Q74/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="T74">
-        <f t="shared" ref="T74:T77" si="54">MOD(ROUNDDOWN((R74/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T74:T77" si="56">MOD(ROUNDDOWN((R74/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U74">
-        <f>IF(S74=T74,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q75">
-        <f t="shared" ref="Q75:Q82" si="55">$Q$73</f>
+        <f t="shared" ref="Q75:Q82" si="57">$Q$73</f>
         <v>7</v>
       </c>
       <c r="R75">
-        <f t="shared" ref="R75:R82" si="56">R74+1</f>
+        <f t="shared" ref="R75:R82" si="58">R74+1</f>
         <v>3</v>
       </c>
       <c r="S75">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>1</v>
       </c>
       <c r="T75">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+      <c r="U75">
         <f t="shared" si="54"/>
-        <v>1</v>
-      </c>
-      <c r="U75">
-        <f>IF(S75=T75,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q76">
+        <f t="shared" si="57"/>
+        <v>7</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="58"/>
+        <v>4</v>
+      </c>
+      <c r="S76">
         <f t="shared" si="55"/>
-        <v>7</v>
-      </c>
-      <c r="R76">
+        <v>1</v>
+      </c>
+      <c r="T76">
         <f t="shared" si="56"/>
-        <v>4</v>
-      </c>
-      <c r="S76">
-        <f t="shared" si="53"/>
-        <v>1</v>
-      </c>
-      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
         <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="U76">
-        <f>IF(S76=T76,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q77">
+        <f t="shared" si="57"/>
+        <v>7</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="58"/>
+        <v>5</v>
+      </c>
+      <c r="S77">
         <f t="shared" si="55"/>
-        <v>7</v>
-      </c>
-      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="T77">
         <f t="shared" si="56"/>
-        <v>5</v>
-      </c>
-      <c r="S77">
-        <f t="shared" si="53"/>
-        <v>1</v>
-      </c>
-      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77">
         <f t="shared" si="54"/>
-        <v>1</v>
-      </c>
-      <c r="U77">
-        <f>IF(S77=T77,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q78">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>7</v>
       </c>
       <c r="R78">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>6</v>
       </c>
       <c r="S78">
@@ -2614,107 +2614,107 @@
       </c>
       <c r="T78">
         <f>MOD(ROUNDDOWN((R78/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78">
-        <f>IF(S78=T78,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q79">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>7</v>
       </c>
       <c r="R79">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>7</v>
       </c>
       <c r="S79">
-        <f t="shared" ref="S79:S82" si="57">MOD(ROUNDDOWN((Q79/$T$9),0),2)</f>
+        <f t="shared" ref="S79:S82" si="59">MOD(ROUNDDOWN((Q79/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="T79">
-        <f t="shared" ref="T79:T82" si="58">MOD(ROUNDDOWN((R79/$T$9),0),2)</f>
+        <f t="shared" ref="T79:T82" si="60">MOD(ROUNDDOWN((R79/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="U79">
-        <f>IF(S79=T79,1,0)</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q80">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>7</v>
       </c>
       <c r="R80">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>8</v>
       </c>
       <c r="S80">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="T80">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="U80">
-        <f>IF(S80=T80,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q81">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>7</v>
       </c>
       <c r="R81">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>9</v>
       </c>
       <c r="S81">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="T81">
-        <f t="shared" si="58"/>
-        <v>1</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="U81">
-        <f>IF(S81=T81,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q82">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>7</v>
       </c>
       <c r="R82">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="S82">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="T82">
-        <f t="shared" si="58"/>
-        <v>0</v>
+        <f t="shared" si="60"/>
+        <v>1</v>
       </c>
       <c r="U82">
-        <f>IF(S82=T82,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q83" s="6">
+      <c r="Q83" s="4">
         <f>$Q$74+1</f>
         <v>8</v>
       </c>
-      <c r="R83" s="4">
+      <c r="R83" s="2">
         <v>1</v>
       </c>
       <c r="S83">
@@ -2723,15 +2723,15 @@
       </c>
       <c r="T83">
         <f>MOD(ROUNDDOWN((R83/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U83">
-        <f>IF(S83=T83,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q84" s="6">
+      <c r="Q84" s="4">
         <f>$Q$83</f>
         <v>8</v>
       </c>
@@ -2740,91 +2740,91 @@
         <v>2</v>
       </c>
       <c r="S84">
-        <f t="shared" ref="S84:S87" si="59">MOD(ROUNDDOWN((Q84/$T$9),0),2)</f>
+        <f t="shared" ref="S84:S87" si="61">MOD(ROUNDDOWN((Q84/$T$9),0),2)</f>
         <v>0</v>
       </c>
       <c r="T84">
-        <f t="shared" ref="T84:T87" si="60">MOD(ROUNDDOWN((R84/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T84:T87" si="62">MOD(ROUNDDOWN((R84/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U84">
-        <f>IF(S84=T84,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q85" s="6">
-        <f t="shared" ref="Q85:Q92" si="61">$Q$83</f>
+      <c r="Q85" s="4">
+        <f t="shared" ref="Q85:Q92" si="63">$Q$83</f>
         <v>8</v>
       </c>
       <c r="R85">
-        <f t="shared" ref="R85:R92" si="62">R84+1</f>
+        <f t="shared" ref="R85:R92" si="64">R84+1</f>
         <v>3</v>
       </c>
       <c r="S85">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="T85">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="U85">
-        <f>IF(S85=T85,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q86" s="6">
+      <c r="Q86" s="4">
+        <f t="shared" si="63"/>
+        <v>8</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="64"/>
+        <v>4</v>
+      </c>
+      <c r="S86">
         <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q87" s="4">
+        <f t="shared" si="63"/>
         <v>8</v>
       </c>
-      <c r="R86">
+      <c r="R87">
+        <f t="shared" si="64"/>
+        <v>5</v>
+      </c>
+      <c r="S87">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="T87">
         <f t="shared" si="62"/>
-        <v>4</v>
-      </c>
-      <c r="S86">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="T86">
-        <f t="shared" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="U86">
-        <f>IF(S86=T86,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q87" s="6">
-        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q88" s="4">
+        <f t="shared" si="63"/>
         <v>8</v>
       </c>
-      <c r="R87">
-        <f t="shared" si="62"/>
-        <v>5</v>
-      </c>
-      <c r="S87">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="T87">
-        <f t="shared" si="60"/>
-        <v>1</v>
-      </c>
-      <c r="U87">
-        <f>IF(S87=T87,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q88" s="6">
-        <f t="shared" si="61"/>
-        <v>8</v>
-      </c>
       <c r="R88">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>6</v>
       </c>
       <c r="S88">
@@ -2833,99 +2833,99 @@
       </c>
       <c r="T88">
         <f>MOD(ROUNDDOWN((R88/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U88">
-        <f>IF(S88=T88,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q89" s="6">
-        <f t="shared" si="61"/>
+      <c r="Q89" s="4">
+        <f t="shared" si="63"/>
         <v>8</v>
       </c>
       <c r="R89">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>7</v>
       </c>
       <c r="S89">
-        <f t="shared" ref="S89:S92" si="63">MOD(ROUNDDOWN((Q89/$T$9),0),2)</f>
+        <f t="shared" ref="S89:S92" si="65">MOD(ROUNDDOWN((Q89/$T$9),0),2)</f>
         <v>0</v>
       </c>
       <c r="T89">
-        <f t="shared" ref="T89:T92" si="64">MOD(ROUNDDOWN((R89/$T$9),0),2)</f>
+        <f t="shared" ref="T89:T92" si="66">MOD(ROUNDDOWN((R89/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="U89">
-        <f>IF(S89=T89,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q90" s="6">
-        <f t="shared" si="61"/>
+      <c r="Q90" s="4">
+        <f t="shared" si="63"/>
         <v>8</v>
       </c>
       <c r="R90">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>8</v>
       </c>
       <c r="S90">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="T90">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q91" s="4">
         <f t="shared" si="63"/>
-        <v>0</v>
-      </c>
-      <c r="T90">
+        <v>8</v>
+      </c>
+      <c r="R91">
         <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="U90">
-        <f>IF(S90=T90,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q91" s="6">
-        <f t="shared" si="61"/>
+        <v>9</v>
+      </c>
+      <c r="S91">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q92" s="4">
+        <f t="shared" si="63"/>
         <v>8</v>
       </c>
-      <c r="R91">
-        <f t="shared" si="62"/>
-        <v>9</v>
-      </c>
-      <c r="S91">
-        <f t="shared" si="63"/>
-        <v>0</v>
-      </c>
-      <c r="T91">
+      <c r="R92">
         <f t="shared" si="64"/>
-        <v>1</v>
-      </c>
-      <c r="U91">
-        <f>IF(S91=T91,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q92" s="6">
-        <f t="shared" si="61"/>
-        <v>8</v>
-      </c>
-      <c r="R92">
-        <f t="shared" si="62"/>
         <v>10</v>
       </c>
       <c r="S92">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="T92">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
       <c r="U92">
-        <f>IF(S92=T92,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="17:21" x14ac:dyDescent="0.25">
@@ -2933,19 +2933,19 @@
         <f>Q83+1</f>
         <v>9</v>
       </c>
-      <c r="R93" s="4">
+      <c r="R93" s="2">
         <v>1</v>
       </c>
       <c r="S93">
         <f>MOD(ROUNDDOWN((Q93/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T93">
         <f>MOD(ROUNDDOWN((R93/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U93">
-        <f>IF(S93=T93,1,0)</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
@@ -2959,196 +2959,196 @@
         <v>2</v>
       </c>
       <c r="S94">
-        <f t="shared" ref="S94:S97" si="65">MOD(ROUNDDOWN((Q94/$T$9),0),2)</f>
-        <v>1</v>
+        <f t="shared" ref="S94:S97" si="67">MOD(ROUNDDOWN((Q94/$T$9),0),2)</f>
+        <v>0</v>
       </c>
       <c r="T94">
-        <f t="shared" ref="T94:T97" si="66">MOD(ROUNDDOWN((R94/$T$9),0),2)</f>
-        <v>0</v>
+        <f t="shared" ref="T94:T97" si="68">MOD(ROUNDDOWN((R94/$T$9),0),2)</f>
+        <v>1</v>
       </c>
       <c r="U94">
-        <f>IF(S94=T94,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q95">
-        <f t="shared" ref="Q95:Q103" si="67">$Q$93</f>
+        <f t="shared" ref="Q95:Q102" si="69">$Q$93</f>
         <v>9</v>
       </c>
       <c r="R95">
-        <f t="shared" ref="R95:R102" si="68">R94+1</f>
+        <f t="shared" ref="R95:R102" si="70">R94+1</f>
         <v>3</v>
       </c>
       <c r="S95">
-        <f t="shared" si="65"/>
-        <v>1</v>
+        <f t="shared" si="67"/>
+        <v>0</v>
       </c>
       <c r="T95">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="U95">
-        <f>IF(S95=T95,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q96">
+        <f t="shared" si="69"/>
+        <v>9</v>
+      </c>
+      <c r="R96">
+        <f t="shared" si="70"/>
+        <v>4</v>
+      </c>
+      <c r="S96">
         <f t="shared" si="67"/>
-        <v>9</v>
-      </c>
-      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="T96">
         <f t="shared" si="68"/>
-        <v>4</v>
-      </c>
-      <c r="S96">
-        <f t="shared" si="65"/>
-        <v>1</v>
-      </c>
-      <c r="T96">
-        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="U96">
-        <f>IF(S96=T96,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q97">
+        <f t="shared" si="69"/>
+        <v>9</v>
+      </c>
+      <c r="R97">
+        <f t="shared" si="70"/>
+        <v>5</v>
+      </c>
+      <c r="S97">
         <f t="shared" si="67"/>
-        <v>9</v>
-      </c>
-      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="T97">
         <f t="shared" si="68"/>
-        <v>5</v>
-      </c>
-      <c r="S97">
-        <f t="shared" si="65"/>
-        <v>1</v>
-      </c>
-      <c r="T97">
-        <f t="shared" si="66"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U97">
-        <f>IF(S97=T97,1,0)</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q98">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>9</v>
       </c>
       <c r="R98">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>6</v>
       </c>
       <c r="S98">
         <f>MOD(ROUNDDOWN((Q98/$T$9),0),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T98">
         <f>MOD(ROUNDDOWN((R98/$T$9),0),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U98">
-        <f>IF(S98=T98,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q99">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>9</v>
       </c>
       <c r="R99">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>7</v>
       </c>
       <c r="S99">
-        <f t="shared" ref="S99:S102" si="69">MOD(ROUNDDOWN((Q99/$T$9),0),2)</f>
-        <v>1</v>
+        <f t="shared" ref="S99:S102" si="71">MOD(ROUNDDOWN((Q99/$T$9),0),2)</f>
+        <v>0</v>
       </c>
       <c r="T99">
-        <f t="shared" ref="T99:T102" si="70">MOD(ROUNDDOWN((R99/$T$9),0),2)</f>
+        <f t="shared" ref="T99:T102" si="72">MOD(ROUNDDOWN((R99/$T$9),0),2)</f>
         <v>1</v>
       </c>
       <c r="U99">
-        <f>IF(S99=T99,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q100">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>9</v>
       </c>
       <c r="R100">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>8</v>
       </c>
       <c r="S100">
-        <f t="shared" si="69"/>
-        <v>1</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="T100">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="U100">
-        <f>IF(S100=T100,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q101">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>9</v>
       </c>
       <c r="R101">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>9</v>
       </c>
       <c r="S101">
-        <f t="shared" si="69"/>
-        <v>1</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="T101">
-        <f t="shared" si="70"/>
-        <v>1</v>
+        <f t="shared" si="72"/>
+        <v>0</v>
       </c>
       <c r="U101">
-        <f>IF(S101=T101,1,0)</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q102">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>9</v>
       </c>
       <c r="R102">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>10</v>
       </c>
       <c r="S102">
-        <f t="shared" si="69"/>
-        <v>1</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="T102">
-        <f t="shared" si="70"/>
-        <v>0</v>
+        <f t="shared" si="72"/>
+        <v>1</v>
       </c>
       <c r="U102">
-        <f>IF(S102=T102,1,0)</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="R103" s="4"/>
+      <c r="R103" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>